<commit_message>
CLC looping unit process
</commit_message>
<xml_diff>
--- a/data/cement/cement_calcs.xlsx
+++ b/data/cement/cement_calcs.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="111">
   <si>
     <t>combustion</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>meal2clinker</t>
+  </si>
+  <si>
+    <t>Fuel</t>
   </si>
 </sst>
 </file>
@@ -1810,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A13" sqref="A13:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2082,7 +2085,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>82</v>
@@ -2112,15 +2115,17 @@
         <v>4</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2131,13 +2136,13 @@
         <v>4</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>36</v>
@@ -2146,10 +2151,10 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>31</v>
@@ -2158,22 +2163,20 @@
         <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>36</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="13" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>4</v>
@@ -2184,99 +2187,80 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1"/>
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>2</v>
+      <c r="C20" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="A21" s="3"/>
+      <c r="B21" t="s">
         <v>83</v>
       </c>
+      <c r="C21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="E21" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="12" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>